<commit_message>
add date and update api-spec.xlsx
</commit_message>
<xml_diff>
--- a/API-spec.xlsx
+++ b/API-spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Projects\2018\Highton_Spirit-In-Motion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888F0FCA-7DED-4A3E-A607-D689D0521EC2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DCF731-E073-43EC-B91B-6D6E8837FBA0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576" tabRatio="540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,20 +193,49 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>writer
+content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문에 대해 답변 씀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장소 얻어오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/place</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 체육시설들을 얻어옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Code: 200
+[
+    {
+        lat: String,
+        lng: String,
+        placeName: String,
+    },
+    ...
+]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Status Code : 200
 [
     {
         id: String
         writer: String
         conent: String
+        date: String
     },
     …
 ]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>writer
-content</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -220,35 +249,8 @@
 {
     writer: String
     content: String
+    date: String
 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>질문에 대해 답변 씀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>장소 얻어오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/place</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 체육시설들을 얻어옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status Code: 200
-[
-    {
-        lat: String,
-        lng: String,
-        placeName: String,
-    },
-    ...
-]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -636,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -751,7 +753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="156.6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" ht="174" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -766,7 +768,7 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>21</v>
@@ -786,7 +788,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>20</v>
@@ -796,7 +798,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="208.8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" ht="226.2" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
@@ -811,7 +813,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>21</v>
@@ -828,10 +830,10 @@
         <v>31</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>20</v>
@@ -842,20 +844,20 @@
     </row>
     <row r="9" spans="1:14" ht="156.6" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>21</v>

</xml_diff>